<commit_message>
Logistic regression to feature scores
</commit_message>
<xml_diff>
--- a/data/Labeled_images.xlsx
+++ b/data/Labeled_images.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roxanadaneshjou/Dropbox/Telederm_photo_quality/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6572A7-9E5B-024C-AA88-F482B884A17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FED0076-1956-CB4E-BBA8-E95FB652DB03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="2520" windowWidth="27240" windowHeight="16440" xr2:uid="{536E09F2-C26B-8E48-AAAE-74F079C69034}"/>
+    <workbookView xWindow="3440" yWindow="3020" windowWidth="27240" windowHeight="16440" xr2:uid="{536E09F2-C26B-8E48-AAAE-74F079C69034}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="200">
   <si>
     <t>gallery_125342_11319_75581.jpg</t>
   </si>
@@ -273,6 +273,366 @@
   </si>
   <si>
     <t>gallery_69512_7594_18488.jpg</t>
+  </si>
+  <si>
+    <t>gallery_98269_9389_6421.jpg</t>
+  </si>
+  <si>
+    <t>gallery_34384_2143_93157.jpg</t>
+  </si>
+  <si>
+    <t>lighting, zoom</t>
+  </si>
+  <si>
+    <t>gallery_43807_3217_19585.jpg</t>
+  </si>
+  <si>
+    <t>gallery_101040_9828_8331.jpg</t>
+  </si>
+  <si>
+    <t>gallery_42993_3112_120496.jpg</t>
+  </si>
+  <si>
+    <t>gallery_71986_7790_236403.jpg</t>
+  </si>
+  <si>
+    <t>gallery_8036_6684_146100.jpg</t>
+  </si>
+  <si>
+    <t>gallery_90779_9571_427837.jpg</t>
+  </si>
+  <si>
+    <t>gallery_112151_10832_8173.jpg</t>
+  </si>
+  <si>
+    <t>gallery_1_6394_69572.jpg</t>
+  </si>
+  <si>
+    <t>gallery_4562_1917_16183.jpg</t>
+  </si>
+  <si>
+    <t>gallery_31353_2354_65495.jpg</t>
+  </si>
+  <si>
+    <t>gallery_31353_2354_16691.jpg</t>
+  </si>
+  <si>
+    <t>gallery_30406_7461_35291.gif</t>
+  </si>
+  <si>
+    <t>gallery_38957_2622_5452.jpg</t>
+  </si>
+  <si>
+    <t>gallery_25955_1363_25912.jpg</t>
+  </si>
+  <si>
+    <t>gallery_116840_10473_24551.jpg</t>
+  </si>
+  <si>
+    <t>gallery_48939_3844_50487.jpg</t>
+  </si>
+  <si>
+    <t>gallery_4562_1917_7565.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_69234.jpg</t>
+  </si>
+  <si>
+    <t>gallery_103765_9919_127305.jpg</t>
+  </si>
+  <si>
+    <t>gallery_23696_2475_61434.jpg</t>
+  </si>
+  <si>
+    <t>gallery_30831_3288_12555.jpg</t>
+  </si>
+  <si>
+    <t>gallery_8036_6684_511996.jpg</t>
+  </si>
+  <si>
+    <t>gallery_61486_6812_249384.jpg</t>
+  </si>
+  <si>
+    <t>gallery_103765_9919_62163.jpg</t>
+  </si>
+  <si>
+    <t>gallery_90779_9571_7772.jpg</t>
+  </si>
+  <si>
+    <t>gallery_30831_3288_59746.jpg</t>
+  </si>
+  <si>
+    <t>gallery_66060_7326_161719.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44736_3344_503099.jpg</t>
+  </si>
+  <si>
+    <t>gallery_57903_6476_7657.jpg</t>
+  </si>
+  <si>
+    <t>gallery_14295_555_1102211051.jpg</t>
+  </si>
+  <si>
+    <t>gallery_8036_6684_528136.jpg</t>
+  </si>
+  <si>
+    <t>gallery_90779_9571_252719.jpg</t>
+  </si>
+  <si>
+    <t>gallery_116840_10473_42685.jpg</t>
+  </si>
+  <si>
+    <t>gallery_23696_2475_103854.jpg</t>
+  </si>
+  <si>
+    <t>lighting, blurry</t>
+  </si>
+  <si>
+    <t>gallery_68139_8829_201328.jpg</t>
+  </si>
+  <si>
+    <t>gallery_90779_9571_266237.jpg</t>
+  </si>
+  <si>
+    <t>gallery_68139_8829_895773.jpg</t>
+  </si>
+  <si>
+    <t>gallery_19962_713_7352.jpg</t>
+  </si>
+  <si>
+    <t>gallery_82738_12229_28127.jpg</t>
+  </si>
+  <si>
+    <t>gallery_35470_2156_296862.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44779_7162_30813.jpg</t>
+  </si>
+  <si>
+    <t>gallery_8036_6684_1567047.jpg</t>
+  </si>
+  <si>
+    <t>gallery_68139_8829_490519.jpg</t>
+  </si>
+  <si>
+    <t>gallery_116840_10473_537005.jpg</t>
+  </si>
+  <si>
+    <t>gallery_75430_8029_1040.jpg</t>
+  </si>
+  <si>
+    <t>gallery_113885_10216_640431.jpg</t>
+  </si>
+  <si>
+    <t>gallery_105071_9762_770785.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63645_7016_4933.jpg</t>
+  </si>
+  <si>
+    <t>gallery_67891_7493_1017.jpg</t>
+  </si>
+  <si>
+    <t>gallery_96053_9246_12114.jpg</t>
+  </si>
+  <si>
+    <t>gallery_35470_2156_151550.jpg</t>
+  </si>
+  <si>
+    <t>gallery_81620_8511_21048.jpg</t>
+  </si>
+  <si>
+    <t>gallery_4562_1917_9174.jpg</t>
+  </si>
+  <si>
+    <t>gallery_78864_8372_460412.jpg</t>
+  </si>
+  <si>
+    <t>gallery_56169_5923_2143.jpg</t>
+  </si>
+  <si>
+    <t>gallery_31353_2354_17560.jpg</t>
+  </si>
+  <si>
+    <t>gallery_61399_7052_223558.jpg</t>
+  </si>
+  <si>
+    <t>gallery_28244_12151_4954.jpg</t>
+  </si>
+  <si>
+    <t>gallery_76469_8555_180153.jpg</t>
+  </si>
+  <si>
+    <t>gallery_31353_2354_5046.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_21144.jpg</t>
+  </si>
+  <si>
+    <t>gallery_105071_9762_113285.jpg</t>
+  </si>
+  <si>
+    <t>gallery_84008_8980_1682903.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63645_7016_6704.jpg</t>
+  </si>
+  <si>
+    <t>gallery_78864_8372_709381.jpg</t>
+  </si>
+  <si>
+    <t>gallery_67891_7493_33715.jpg</t>
+  </si>
+  <si>
+    <t>gallery_69749_7569_59711.jpg</t>
+  </si>
+  <si>
+    <t>gallery_101577_9580_29919.jpg</t>
+  </si>
+  <si>
+    <t>gallery_54421_5842_39054.jpg</t>
+  </si>
+  <si>
+    <t>gallery_99103_9419_110971.jpg</t>
+  </si>
+  <si>
+    <t>gallery_93094_9517_154094.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44173_3278_5181.jpg</t>
+  </si>
+  <si>
+    <t>gallery_76469_8555_132641.jpg</t>
+  </si>
+  <si>
+    <t>gallery_66463_7447_4202.jpg</t>
+  </si>
+  <si>
+    <t>gallery_113893_10222_8539.jpg</t>
+  </si>
+  <si>
+    <t>gallery_100309_9486_25714.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_36214.jpg</t>
+  </si>
+  <si>
+    <t>gallery_36262_2241_555718.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44173_3278_10142.jpg</t>
+  </si>
+  <si>
+    <t>gallery_78864_8372_155116.jpg</t>
+  </si>
+  <si>
+    <t>gallery_62541_6903_132665.jpg</t>
+  </si>
+  <si>
+    <t>gallery_61399_7052_77437.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_38361.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_13899.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63645_7016_4713.jpg</t>
+  </si>
+  <si>
+    <t>gallery_63458_7459_22488.jpg</t>
+  </si>
+  <si>
+    <t>gallery_94299_9154_130157.jpg</t>
+  </si>
+  <si>
+    <t>gallery_67891_7493_37819.jpg</t>
+  </si>
+  <si>
+    <t>gallery_105071_9762_613032.jpg</t>
+  </si>
+  <si>
+    <t>gallery_82851_8574_60991.jpg</t>
+  </si>
+  <si>
+    <t>gallery_35360_2532_29675.jpg</t>
+  </si>
+  <si>
+    <t>gallery_106043_9821_22998.jpg</t>
+  </si>
+  <si>
+    <t>gallery_111232_10090_8273.jpg</t>
+  </si>
+  <si>
+    <t>gallery_36350_2268_269970.jpg</t>
+  </si>
+  <si>
+    <t>gallery_96265_9375_955.jpg</t>
+  </si>
+  <si>
+    <t>gallery_67891_7493_72765.jpg</t>
+  </si>
+  <si>
+    <t>gallery_81620_8511_12641.jpg</t>
+  </si>
+  <si>
+    <t>gallery_61399_7052_95470.jpg</t>
+  </si>
+  <si>
+    <t>gallery_125459_10784_434216.jpg</t>
+  </si>
+  <si>
+    <t>gallery_110090_10537_55606.jpg</t>
+  </si>
+  <si>
+    <t>gallery_35470_2156_23507.jpg</t>
+  </si>
+  <si>
+    <t>gallery_105601_9803_1274466.jpg</t>
+  </si>
+  <si>
+    <t>gallery_62541_6903_32097.jpg</t>
+  </si>
+  <si>
+    <t>gallery_36262_2241_994045.jpg</t>
+  </si>
+  <si>
+    <t>gallery_42513_3056_237816.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44736_3344_6253.jpg</t>
+  </si>
+  <si>
+    <t>gallery_36752_3083_192353.jpg</t>
+  </si>
+  <si>
+    <t>gallery_98033_9382_107966.jpg</t>
+  </si>
+  <si>
+    <t>gallery_45741_3481_36398.jpg</t>
+  </si>
+  <si>
+    <t>gallery_44779_7162_15587.jpg</t>
+  </si>
+  <si>
+    <t>gallery_35360_2532_7566.jpg</t>
+  </si>
+  <si>
+    <t>gallery_36350_2268_1018247.jpg</t>
+  </si>
+  <si>
+    <t>gallery_123853_10646_57657.jpg</t>
+  </si>
+  <si>
+    <t>gallery_117819_11358_9530.jpg</t>
+  </si>
+  <si>
+    <t>gallery_18613_649_1105665586.jpg</t>
+  </si>
+  <si>
+    <t>gallery_60039_6675_537645.jpg</t>
   </si>
 </sst>
 </file>
@@ -632,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E703979-3945-D445-A0E5-E4A69F902399}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="117" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1435,6 +1795,1414 @@
         <v>3</v>
       </c>
     </row>
+    <row r="73" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B74" t="s">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1</v>
+      </c>
+      <c r="C75" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B77" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B79" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B80" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B85" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" t="s">
+        <v>1</v>
+      </c>
+      <c r="C86" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="C87" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B88" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B89" t="s">
+        <v>1</v>
+      </c>
+      <c r="C89" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B90" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B91" t="s">
+        <v>5</v>
+      </c>
+      <c r="C91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A92" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" t="s">
+        <v>1</v>
+      </c>
+      <c r="C92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A93" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A94" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A95" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B95" t="s">
+        <v>1</v>
+      </c>
+      <c r="C95" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A96" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A97" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B97" t="s">
+        <v>1</v>
+      </c>
+      <c r="C97" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A98" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B98" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A99" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B99" t="s">
+        <v>1</v>
+      </c>
+      <c r="C99" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A100" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C100" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A101" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A102" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A103" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A104" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A105" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" t="s">
+        <v>5</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A106" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A107" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B107" t="s">
+        <v>5</v>
+      </c>
+      <c r="C107" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A108" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A109" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A110" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B110" t="s">
+        <v>5</v>
+      </c>
+      <c r="C110" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B114" t="s">
+        <v>5</v>
+      </c>
+      <c r="C114" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C116" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A117" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B117" t="s">
+        <v>1</v>
+      </c>
+      <c r="C117" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A118" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B118" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A119" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B119" t="s">
+        <v>1</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A120" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B120" t="s">
+        <v>1</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A121" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B121" t="s">
+        <v>5</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A122" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B122" t="s">
+        <v>1</v>
+      </c>
+      <c r="C122" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A123" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B123" t="s">
+        <v>5</v>
+      </c>
+      <c r="C123" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A124" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B125" t="s">
+        <v>5</v>
+      </c>
+      <c r="C125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B126" t="s">
+        <v>5</v>
+      </c>
+      <c r="C126" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B127" t="s">
+        <v>5</v>
+      </c>
+      <c r="C127" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A128" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C128" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A129" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B129" t="s">
+        <v>1</v>
+      </c>
+      <c r="C129" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A130" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C130" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A131" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B131" t="s">
+        <v>1</v>
+      </c>
+      <c r="C131" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A132" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B132" t="s">
+        <v>5</v>
+      </c>
+      <c r="C132" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A133" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B133" t="s">
+        <v>1</v>
+      </c>
+      <c r="C133" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B134" t="s">
+        <v>1</v>
+      </c>
+      <c r="C134" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B135" t="s">
+        <v>5</v>
+      </c>
+      <c r="C135" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B136" t="s">
+        <v>1</v>
+      </c>
+      <c r="C136" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B137" t="s">
+        <v>5</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B138" t="s">
+        <v>5</v>
+      </c>
+      <c r="C138" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B139" t="s">
+        <v>5</v>
+      </c>
+      <c r="C139" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A140" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B140" t="s">
+        <v>1</v>
+      </c>
+      <c r="C140" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A141" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B141" t="s">
+        <v>1</v>
+      </c>
+      <c r="C141" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B142" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A143" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B143" t="s">
+        <v>1</v>
+      </c>
+      <c r="C143" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A144" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B144" t="s">
+        <v>1</v>
+      </c>
+      <c r="C144" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A145" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B145" t="s">
+        <v>5</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A146" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B146" t="s">
+        <v>1</v>
+      </c>
+      <c r="C146" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A147" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B147" t="s">
+        <v>1</v>
+      </c>
+      <c r="C147" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A148" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B148" t="s">
+        <v>5</v>
+      </c>
+      <c r="C148" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A149" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B149" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A150" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A151" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B151" t="s">
+        <v>1</v>
+      </c>
+      <c r="C151" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A152" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B152" t="s">
+        <v>1</v>
+      </c>
+      <c r="C152" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A153" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B153" t="s">
+        <v>1</v>
+      </c>
+      <c r="C153" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A154" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B154" t="s">
+        <v>1</v>
+      </c>
+      <c r="C154" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A155" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A156" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B156" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A157" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B157" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A158" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B158" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A159" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B159" t="s">
+        <v>1</v>
+      </c>
+      <c r="C159" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A160" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B160" t="s">
+        <v>1</v>
+      </c>
+      <c r="C160" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A161" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B161" t="s">
+        <v>5</v>
+      </c>
+      <c r="C161" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A162" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B162" t="s">
+        <v>5</v>
+      </c>
+      <c r="C162" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A163" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B163" t="s">
+        <v>1</v>
+      </c>
+      <c r="C163" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A164" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B164" t="s">
+        <v>1</v>
+      </c>
+      <c r="C164" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A165" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B165" t="s">
+        <v>5</v>
+      </c>
+      <c r="C165" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A166" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B166" t="s">
+        <v>1</v>
+      </c>
+      <c r="C166" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A167" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B167" t="s">
+        <v>5</v>
+      </c>
+      <c r="C167" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A168" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B168" t="s">
+        <v>1</v>
+      </c>
+      <c r="C168" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A169" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B169" t="s">
+        <v>1</v>
+      </c>
+      <c r="C169" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A170" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B170" t="s">
+        <v>5</v>
+      </c>
+      <c r="C170" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A171" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B171" t="s">
+        <v>1</v>
+      </c>
+      <c r="C171" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A172" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B172" t="s">
+        <v>5</v>
+      </c>
+      <c r="C172" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A173" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B173" t="s">
+        <v>1</v>
+      </c>
+      <c r="C173" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A174" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B174" t="s">
+        <v>1</v>
+      </c>
+      <c r="C174" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A175" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B175" t="s">
+        <v>5</v>
+      </c>
+      <c r="C175" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A176" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B176" t="s">
+        <v>5</v>
+      </c>
+      <c r="C176" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A177" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B177" t="s">
+        <v>1</v>
+      </c>
+      <c r="C177" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A178" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B178" t="s">
+        <v>1</v>
+      </c>
+      <c r="C178" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A179" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B179" t="s">
+        <v>5</v>
+      </c>
+      <c r="C179" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A180" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B180" t="s">
+        <v>5</v>
+      </c>
+      <c r="C180" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B181" t="s">
+        <v>5</v>
+      </c>
+      <c r="C181" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A182" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B182" t="s">
+        <v>5</v>
+      </c>
+      <c r="C182" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A183" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B183" t="s">
+        <v>5</v>
+      </c>
+      <c r="C183" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A184" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B184" t="s">
+        <v>5</v>
+      </c>
+      <c r="C184" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A185" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B185" t="s">
+        <v>1</v>
+      </c>
+      <c r="C185" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A186" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B186" t="s">
+        <v>5</v>
+      </c>
+      <c r="C186" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A187" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B187" t="s">
+        <v>5</v>
+      </c>
+      <c r="C187" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A188" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B188" t="s">
+        <v>5</v>
+      </c>
+      <c r="C188" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A189" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B189" t="s">
+        <v>5</v>
+      </c>
+      <c r="C189" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A190" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B190" t="s">
+        <v>1</v>
+      </c>
+      <c r="C190" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A191" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B191" t="s">
+        <v>1</v>
+      </c>
+      <c r="C191" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A192" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B192" t="s">
+        <v>1</v>
+      </c>
+      <c r="C192" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A193" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1</v>
+      </c>
+      <c r="C193" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A194" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B194" t="s">
+        <v>5</v>
+      </c>
+      <c r="C194" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A195" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B195" t="s">
+        <v>5</v>
+      </c>
+      <c r="C195" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A196" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B196" t="s">
+        <v>5</v>
+      </c>
+      <c r="C196" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A197" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B197" t="s">
+        <v>1</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A198" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B198" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A199" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B199" t="s">
+        <v>1</v>
+      </c>
+      <c r="C199" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A200" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>